<commit_message>
Change and XLSX file header to year to include it in join. Update travis. Use mat64 to calculate hypothesis
</commit_message>
<xml_diff>
--- a/res/S&PStockPrices.xlsx
+++ b/res/S&PStockPrices.xlsx
@@ -26,10 +26,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Date</t>
+    <t>Price</t>
   </si>
   <si>
-    <t>Price</t>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -119,8 +119,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -431,9 +459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -443,10 +469,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75">
       <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>